<commit_message>
created first data wrangling pipeline
</commit_message>
<xml_diff>
--- a/data/airmonitors_addresses.xlsx
+++ b/data/airmonitors_addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilshah/Desktop/R Files/R Working Directory/RRC_IQAir/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E4B3BF-70FC-DA42-9D9A-1D588618EE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB0AACF-7391-5048-BB48-FFE8421060A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28180" windowHeight="16340" xr2:uid="{5E6ADD94-4CA5-0840-BDA9-D94A5126F3E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
   <si>
     <t>36C0Y29KQGW</t>
   </si>
@@ -306,13 +306,37 @@
   </si>
   <si>
     <t>1477 W Orchard Street</t>
+  </si>
+  <si>
+    <t>9PXQSCXCDQO</t>
+  </si>
+  <si>
+    <t>5J5PWHMBZTG</t>
+  </si>
+  <si>
+    <t>4Y4P2KB4PQD</t>
+  </si>
+  <si>
+    <t>P3E1UGG1272</t>
+  </si>
+  <si>
+    <t>GM5BWS8UMEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983 N Lilac Ave </t>
+  </si>
+  <si>
+    <t>8550 Sierra Ave</t>
+  </si>
+  <si>
+    <t>4870 Thornbush Way</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,6 +361,12 @@
       <sz val="12"/>
       <color rgb="FF202124"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -700,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1886CC-F039-6C42-82A5-598C9FA3D1D0}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,102 +773,78 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>60</v>
+        <v>96</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>66</v>
@@ -846,45 +852,33 @@
       <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>60</v>
@@ -892,6 +886,7 @@
       <c r="E8" t="s">
         <v>53</v>
       </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="J8" s="3"/>
@@ -904,17 +899,18 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="J9" s="3"/>
@@ -927,11 +923,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
       </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -942,13 +946,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -965,13 +969,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -988,10 +992,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>60</v>
@@ -1011,13 +1015,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
         <v>54</v>
@@ -1034,16 +1038,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1057,13 +1055,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>54</v>
@@ -1076,16 +1074,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1095,16 +1093,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1114,10 +1112,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>60</v>
@@ -1133,10 +1131,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>66</v>
@@ -1152,10 +1150,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1163,16 +1167,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1184,10 +1188,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1197,16 +1207,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1218,16 +1228,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1239,13 +1249,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
@@ -1260,13 +1264,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
@@ -1281,13 +1285,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
         <v>53</v>
@@ -1300,16 +1298,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1319,10 +1317,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1330,13 +1334,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E31" t="s">
         <v>53</v>
@@ -1349,13 +1353,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E32" t="s">
         <v>54</v>
@@ -1368,13 +1372,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
         <v>53</v>
@@ -1387,13 +1391,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E34" t="s">
         <v>54</v>
@@ -1406,16 +1410,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1425,16 +1423,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1444,16 +1442,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1463,16 +1461,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1482,16 +1480,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -1501,16 +1499,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -1520,7 +1518,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="E41" t="s">
         <v>54</v>
@@ -1531,10 +1535,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>66</v>
@@ -1550,10 +1554,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>66</v>
@@ -1569,13 +1573,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E44" t="s">
         <v>53</v>
@@ -1588,13 +1592,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
         <v>54</v>
@@ -1607,13 +1611,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="E46" t="s">
         <v>54</v>
@@ -1626,16 +1624,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="4"/>
@@ -1645,10 +1643,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1656,16 +1660,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -1675,13 +1679,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E50" t="s">
         <v>54</v>
@@ -1694,16 +1698,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -1713,12 +1717,12 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D52" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E52" t="s">
@@ -1731,14 +1735,8 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>66</v>
+      <c r="B53" t="s">
+        <v>46</v>
       </c>
       <c r="E53" t="s">
         <v>53</v>
@@ -1751,13 +1749,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E54" t="s">
         <v>54</v>
@@ -1765,7 +1763,93 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>